<commit_message>
A05 v0.1: Completed 1 passenger test (View available event summary)
</commit_message>
<xml_diff>
--- a/test/CruiseActivityManagement/model/pastDateValidations.xlsx
+++ b/test/CruiseActivityManagement/model/pastDateValidations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\eclipse-workspace-ee\CruiseActivityManagement\test\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\eclipse-workspace-ee\CruiseActivityManagement\test\CruiseActivityManagement\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371CE988-26FE-4109-BFF5-1FF0ED69588F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2FD128-464A-404A-98E4-601AF49F1036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,42 +36,42 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={2B006F5F-D001-4821-BC15-870546E0FF28}</author>
-    <author>tc={08E4F5E9-AA2B-4862-9707-3F38BF55D652}</author>
-    <author>tc={B12117AB-7FF9-4C80-9FE7-338B6B3888A6}</author>
-    <author>tc={AA8E1672-82FC-47D9-8CC7-3D436797C56A}</author>
+    <author>tc={32292F77-DB3A-4919-941C-DC49A46E98E5}</author>
+    <author>tc={62D7D2E1-3F64-46A0-BC11-150171F95099}</author>
+    <author>tc={802D12E5-F410-4BAB-9ABE-5262236B71A7}</author>
+    <author>tc={62146368-0E3E-4BCA-B272-A696D4D5468C}</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{2B006F5F-D001-4821-BC15-870546E0FF28}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{32292F77-DB3A-4919-941C-DC49A46E98E5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Current time -1 minute</t>
+    -1 minute from 10/7/20 (boundary value)</t>
       </text>
     </comment>
-    <comment ref="A4" authorId="1" shapeId="0" xr:uid="{08E4F5E9-AA2B-4862-9707-3F38BF55D652}">
+    <comment ref="A4" authorId="1" shapeId="0" xr:uid="{62D7D2E1-3F64-46A0-BC11-150171F95099}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    current date - 1 day</t>
+    0 minutes from 10/7/20 (boundary value)</t>
       </text>
     </comment>
-    <comment ref="A5" authorId="2" shapeId="0" xr:uid="{B12117AB-7FF9-4C80-9FE7-338B6B3888A6}">
+    <comment ref="A5" authorId="2" shapeId="0" xr:uid="{802D12E5-F410-4BAB-9ABE-5262236B71A7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Current time + 1 minute</t>
+    boundary value where events exist</t>
       </text>
     </comment>
-    <comment ref="A6" authorId="3" shapeId="0" xr:uid="{AA8E1672-82FC-47D9-8CC7-3D436797C56A}">
+    <comment ref="A6" authorId="3" shapeId="0" xr:uid="{62146368-0E3E-4BCA-B272-A696D4D5468C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Current date +1 date</t>
+    Extreme value (past)</t>
       </text>
     </comment>
   </commentList>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>test case no</t>
   </si>
@@ -121,13 +121,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\/d\/yy\ hh:mm"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -525,17 +531,17 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A3" dT="2020-10-28T21:53:48.70" personId="{068837F4-5541-422E-B699-9E125C2AEDAA}" id="{2B006F5F-D001-4821-BC15-870546E0FF28}">
-    <text>Current time -1 minute</text>
+  <threadedComment ref="A3" dT="2020-11-15T18:37:12.20" personId="{068837F4-5541-422E-B699-9E125C2AEDAA}" id="{32292F77-DB3A-4919-941C-DC49A46E98E5}">
+    <text>-1 minute from 10/7/20 (boundary value)</text>
   </threadedComment>
-  <threadedComment ref="A4" dT="2020-10-28T21:54:08.77" personId="{068837F4-5541-422E-B699-9E125C2AEDAA}" id="{08E4F5E9-AA2B-4862-9707-3F38BF55D652}">
-    <text>current date - 1 day</text>
+  <threadedComment ref="A4" dT="2020-11-15T18:37:48.65" personId="{068837F4-5541-422E-B699-9E125C2AEDAA}" id="{62D7D2E1-3F64-46A0-BC11-150171F95099}">
+    <text>0 minutes from 10/7/20 (boundary value)</text>
   </threadedComment>
-  <threadedComment ref="A5" dT="2020-10-28T21:54:30.20" personId="{068837F4-5541-422E-B699-9E125C2AEDAA}" id="{B12117AB-7FF9-4C80-9FE7-338B6B3888A6}">
-    <text>Current time + 1 minute</text>
+  <threadedComment ref="A5" dT="2020-11-15T18:40:06.71" personId="{068837F4-5541-422E-B699-9E125C2AEDAA}" id="{802D12E5-F410-4BAB-9ABE-5262236B71A7}">
+    <text>boundary value where events exist</text>
   </threadedComment>
-  <threadedComment ref="A6" dT="2020-10-28T21:54:48.67" personId="{068837F4-5541-422E-B699-9E125C2AEDAA}" id="{AA8E1672-82FC-47D9-8CC7-3D436797C56A}">
-    <text>Current date +1 date</text>
+  <threadedComment ref="A6" dT="2020-11-15T18:43:58.95" personId="{068837F4-5541-422E-B699-9E125C2AEDAA}" id="{62146368-0E3E-4BCA-B272-A696D4D5468C}">
+    <text>Extreme value (past)</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -545,7 +551,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,15 +600,18 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ref="B3:B5" ca="1" si="0">NOW()</f>
-        <v>44133.001990625002</v>
+        <f>DATE(20, 10, 6)</f>
+        <v>7585</v>
       </c>
       <c r="C3" s="2">
-        <f ca="1">NOW() - TIME(0,1,0)</f>
-        <v>44133.001296180555</v>
+        <f>DATE(20, 10, 6) + TIME(12,59,0)</f>
+        <v>7585.5409722222221</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -613,21 +622,12 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <f ca="1">NOW()-1</f>
-        <v>44132.001990625002</v>
+        <f>DATE(20, 10, 7)</f>
+        <v>7586</v>
       </c>
       <c r="C4" s="2">
-        <f ca="1">NOW()-1</f>
-        <v>44132.001990625002</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
+        <f>DATE(20, 10, 7) + TIME(0,0,0)</f>
+        <v>7586</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -635,12 +635,12 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>44133.001990625002</v>
+        <f>DATE(20, 10, 8)</f>
+        <v>7587</v>
       </c>
       <c r="C5" s="2">
-        <f ca="1">NOW() + TIME(0,1,0)</f>
-        <v>44133.002685069448</v>
+        <f>DATE(20, 10, 8) + TIME(15,0,0)</f>
+        <v>7587.625</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -648,12 +648,21 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <f ca="1">NOW()+1</f>
-        <v>44134.001990625002</v>
+        <f>DATE(20, 1, 1)</f>
+        <v>7306</v>
       </c>
       <c r="C6" s="2">
-        <f ca="1">NOW()+1</f>
-        <v>44134.001990625002</v>
+        <f>DATE(20, 1, 1)</f>
+        <v>7306</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -664,9 +673,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B4" formula="1"/>
-  </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>